<commit_message>
update db and some function
</commit_message>
<xml_diff>
--- a/backend/Data/danh_sach_co_so.xlsx
+++ b/backend/Data/danh_sach_co_so.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHU DANG PHU\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Healthy-First\backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EFCA5D-1C71-4E2D-BCCF-FBDABD8C91B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9787EDE-2734-4DE5-AA77-C4FD6405DE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91A9D7E8-CDE5-493E-8819-EBF184160022}"/>
+    <workbookView minimized="1" xWindow="5100" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{91A9D7E8-CDE5-493E-8819-EBF184160022}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="9">
   <si>
     <t>efe</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>ewfefew</t>
+  </si>
+  <si>
+    <t>hong ha</t>
+  </si>
+  <si>
+    <t>trung quocs</t>
   </si>
 </sst>
 </file>
@@ -409,17 +415,17 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>

</xml_diff>